<commit_message>
Removed E2s sheet - do not have this data
</commit_message>
<xml_diff>
--- a/Helper Scripts/Methodology.xlsx
+++ b/Helper Scripts/Methodology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccallum.martin\Documents\R_WORK\Child_Poverty_Map\cpov_map_update_complete\CPAF_Dashboard\Helper Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Unmet-Need-Dashboard\Helper Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E76178A-DDF3-4988-AB35-0101B6B8E647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA7DA87-C267-4FFC-806B-2CD7FF1F8AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Education Maintenance Allowance" sheetId="3" r:id="rId4"/>
     <sheet name="Universal Credit" sheetId="4" r:id="rId5"/>
     <sheet name="Money and Welfare Advice" sheetId="7" r:id="rId6"/>
-    <sheet name="Eligible  2s" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>Dataset</t>
   </si>
@@ -214,12 +213,6 @@
 </t>
   </si>
   <si>
-    <t>Eligible Two Year Olds</t>
-  </si>
-  <si>
-    <t>add text here</t>
-  </si>
-  <si>
     <t>Money and Welfare Advice dataset is displayed as 2025.</t>
   </si>
   <si>
@@ -273,7 +266,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,18 +666,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.08203125" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
     <col min="2" max="2" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="126">
+    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -692,7 +685,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="52" customHeight="1">
+    <row r="3" spans="1:2" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -700,7 +693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="378">
+    <row r="4" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -708,10 +701,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" ht="14.5">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" s="5"/>
     </row>
   </sheetData>
@@ -728,13 +721,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -742,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -750,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -758,7 +751,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -766,31 +759,31 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="84">
+    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="70">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="182">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -811,13 +804,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.25" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -833,7 +826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -841,7 +834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -849,7 +842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="98">
+    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -857,23 +850,23 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="84">
+    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="42">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="140">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -894,13 +887,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.75" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -916,7 +909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -924,7 +917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -932,31 +925,31 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="140">
+    <row r="5" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="112">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="70">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="168">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -973,17 +966,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33D3663-F625-404D-9F9A-618D4533EF37}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +984,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -999,7 +992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1007,7 +1000,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1008,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="84">
+    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1023,28 +1016,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28">
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="238">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1056,17 +1049,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3050DF-A96B-49A4-A08C-2F6CF3F579AA}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="13.58203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -1074,7 +1067,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1082,7 +1075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1083,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1098,7 +1091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="238">
+    <row r="5" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1099,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="224">
+    <row r="6" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1114,97 +1107,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02355CEA-B782-4497-9D9F-C73FC5FCE064}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="1" width="17.9140625" customWidth="1"/>
-    <col min="2" max="2" width="16.9140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1452,15 +1365,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="52e19a84-ae27-4b86-a170-8f47b74f4ad2">
@@ -1469,6 +1373,15 @@
     <TaxCatchAll xmlns="435c4395-9d6a-43e2-b03c-3e7c562397ed" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1491,14 +1404,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477E5E9F-C34A-4BDA-BA59-CD79D5669950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7969E561-3058-4957-B9CB-032DD36D40C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1507,4 +1412,12 @@
     <ds:schemaRef ds:uri="435c4395-9d6a-43e2-b03c-3e7c562397ed"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477E5E9F-C34A-4BDA-BA59-CD79D5669950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated to change instances of '...expected uptake' to '...estimated uptake'
</commit_message>
<xml_diff>
--- a/Helper Scripts/Methodology.xlsx
+++ b/Helper Scripts/Methodology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\Unmet-Need-Dashboard\Helper Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccallum.martin\Documents\R_WORK\Child_Poverty_Map\cpov_map_update_complete\CPAF_Dashboard\Helper Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA7DA87-C267-4FFC-806B-2CD7FF1F8AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FF6A74-4FFA-4C9B-AF18-EFCAF52B79ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Education Maintenance Allowance" sheetId="3" r:id="rId4"/>
     <sheet name="Universal Credit" sheetId="4" r:id="rId5"/>
     <sheet name="Money and Welfare Advice" sheetId="7" r:id="rId6"/>
+    <sheet name="Eligible  2s" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="57">
   <si>
     <t>Dataset</t>
   </si>
@@ -127,14 +128,7 @@
     <t>Data</t>
   </si>
   <si>
-    <t>Modelling expected uptake</t>
-  </si>
-  <si>
     <t>Datasets</t>
-  </si>
-  <si>
-    <t>This dashboard aims to support users to identify local areas where there may be unmet need in relation to child poverty. Unmet need is defined as cases where families eligible for support, such as social security, do not access this. 
-The dashboard  highlights data zones that may have unmet need. That is, it highlights areas where the actual rates of uptake for benefits and support related to child poverty differ significantly from modelled expected  uptake of these.</t>
   </si>
   <si>
     <t xml:space="preserve">Financial Vulnerability Index. The index is calculated using three datasets: Council Tax Arrears, Foodbank uptake and Housing Arrears. A rate is calculated using households with children for Foodbank and Housing Arrears datasets. For Council Tax Arrears, a rate is calculated using total number of households as this dataset is only available for all households in arrears. It is then down-weighted when calculating the index to reduce bias. </t>
@@ -170,8 +164,81 @@
     <t>The dashboard contains a combination of council held and publicly available datasets. The data is anonymised and aggregated to data zone level. Prior to modelling, data is converted to rates.</t>
   </si>
   <si>
+    <t xml:space="preserve">Ages 10-18 have been selected as the age groups most likely to be in Primary 6 and above. Children in Primaries 1 to 5 receive a universal entitlement. This does mean some children aged 9 who are in Primary 6 will not included in the data.
+Mid-Year Estimate data does not cover academic years, so there is a slight discrepancy between this and the FSM data. This means rates are not exact.
+Anonymised data was shared at postcode and aggregated to data zone level.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid-Year Estimate data does not cover academic years, so there is a slight discrepancy between this and the Clothing Grant data. This means rates are not exact.
+Anonymised data was shared at postcode and aggregated to data zone level.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mid-Year Estimate data does not cover academic years, so there is a slight discrepancy between this and the EMA data. This means rates are not exact.
+Anonymised data was shared at postcode and aggregated to data zone level.
+</t>
+  </si>
+  <si>
+    <t>Eligible Two Year Olds</t>
+  </si>
+  <si>
+    <t>add text here</t>
+  </si>
+  <si>
+    <t>Money and Welfare Advice dataset is displayed as 2025.</t>
+  </si>
+  <si>
+    <t>Clothing Grant for 2022/23 is displayed as 2023 and for 2024/2025 it is displayed as 2025.</t>
+  </si>
+  <si>
+    <t>Free School Meals for 2022/23 is displayed as 2023 and for 2024/2025 it is displayed as 2025.</t>
+  </si>
+  <si>
+    <t>Education Maintenance Allowance for 2022/23 is displayed as 2023 and for 2024/2025 it is displayed as 2025.</t>
+  </si>
+  <si>
+    <t>Free School Meals: Supplied by West Lothian Council from the SEEMiS database.
+Children in Low Income Families: Accessed from DWP Statxplore.
+Mid Year Population Estimates: National Records of Scotland</t>
+  </si>
+  <si>
+    <t>Free School Meals: Academic years: 2022/23 and 2024/25
+Children in Low Income Families: 2022/23 and 2024/25
+Mid-Year Population Estimates: 2022</t>
+  </si>
+  <si>
+    <t>Clothing Grant: Academic years: 2022/23 and 2024/25
+Children in Low Income Families: 2022/23 and 2024/25
+Mid-Year Population Estimates: 2022</t>
+  </si>
+  <si>
+    <t>Education Maintenance Allowance: Supplied by West Lothian Council from the SEEMiS database.
+Children in Low Income Families: Accessed from DWP Statxplore.
+Mid Year Population Estimates: National Records of Scotland</t>
+  </si>
+  <si>
+    <t>Education Maintenance Allowance: Academic years: 2022/23 and 2024/25
+Children in Low Income Families: 2022/23 and 2024/25
+Mid-Year Population Estimates: 2022</t>
+  </si>
+  <si>
+    <t>Universal Credit: 2025
+Census: 2022</t>
+  </si>
+  <si>
+    <t>Universal Credit data is displayed as 2025.</t>
+  </si>
+  <si>
+    <t>This dashboard aims to support users to identify local areas where there may be unmet need in relation to child poverty. Unmet need is defined as cases where families eligible for support, such as social security, do not access this. 
+The dashboard  highlights data zones that may have unmet need. That is, it highlights areas where the actual rates of uptake for benefits and support related to child poverty differ significantly from modelled estimated  uptake of these.</t>
+  </si>
+  <si>
+    <t>Modelling estimated uptake</t>
+  </si>
+  <si>
     <r>
-      <t>To model e</t>
+      <t>To model estimated</t>
     </r>
     <r>
       <rPr>
@@ -181,7 +248,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">xpected uptake, pairs of measures are used, with each pairing including an “uptake” measure and a “demand” measure. The uptake measure is the benefit or service of interest, and the demand measure is a suitable comparator which can be used to estimate expected uptake. For example, uptake of Free School Meals for children aged 10 to 18 years is used as an uptake measure and the proportion of children aged 10 to 18 years in low-income families is used as a comparative measure of demand. Each pairing of uptake and demand measures have similar eligibility requirements and therefore a linear relationship, meaning that higher rates of demand are typically associated with higher rates of uptake. This relationship can be used to estimate demand.
+      <t xml:space="preserve"> uptake, pairs of measures are used, with each pairing including an “uptake” measure and a “demand” measure. The uptake measure is the benefit or service of interest, and the demand measure is a suitable comparator which can be used to estimate uptake. For example, uptake of Free School Meals for children aged 10 to 18 years is used as an uptake measure and the proportion of children aged 10 to 18 years in low-income families is used as a comparative measure of demand. Each pairing of uptake and demand measures have similar eligibility requirements and therefore a linear relationship, meaning that higher rates of demand are typically associated with higher rates of uptake. This relationship can be used to estimate demand.
  </t>
     </r>
     <r>
@@ -192,81 +259,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>A linear regression model is fitted between each uptake measure and its associated demand measure. The regression model calculates for each data zone what the expected uptake rate would be given the demand rate. Residual values - the difference between the observed rate and the expected rate - are calculated and then standardised. Data zones where the standardised residual is above 2 or below minus 2 are then highlighted in the dashboard as areas where uptake differs from what is expected.  
-When interpreting higher/lower than expected uptake, the expected value does not mean that this is what the rate should be but is the rate most likely at the associated demand rate within the model. In practice, uptake rates will be higher or lower than the modelled values for a range of reasons. </t>
+      <t>A linear regression model is fitted between each uptake measure and its associated demand measure. The regression model calculates for each data zone what the estimated uptake rate would be given the demand rate. Residual values - the difference between the observed rate and the estimated rate - are calculated and then standardised. Data zones where the standardised residual is above 2 or below minus 2 are then highlighted in the dashboard as areas where uptake differs from what is estimated.  
+When interpreting higher/lower than estimated uptake, the estimated value does not mean that this is what the rate should be but is the rate most likely at the associated demand rate within the model. In practice, uptake rates will be higher or lower than the modelled values for a range of reasons. </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Ages 10-18 have been selected as the age groups most likely to be in Primary 6 and above. Children in Primaries 1 to 5 receive a universal entitlement. This does mean some children aged 9 who are in Primary 6 will not included in the data.
-Mid-Year Estimate data does not cover academic years, so there is a slight discrepancy between this and the FSM data. This means rates are not exact.
-Anonymised data was shared at postcode and aggregated to data zone level.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mid-Year Estimate data does not cover academic years, so there is a slight discrepancy between this and the Clothing Grant data. This means rates are not exact.
-Anonymised data was shared at postcode and aggregated to data zone level.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mid-Year Estimate data does not cover academic years, so there is a slight discrepancy between this and the EMA data. This means rates are not exact.
-Anonymised data was shared at postcode and aggregated to data zone level.
-</t>
-  </si>
-  <si>
-    <t>Money and Welfare Advice dataset is displayed as 2025.</t>
-  </si>
-  <si>
-    <t>Clothing Grant for 2022/23 is displayed as 2023 and for 2024/2025 it is displayed as 2025.</t>
-  </si>
-  <si>
-    <t>Free School Meals for 2022/23 is displayed as 2023 and for 2024/2025 it is displayed as 2025.</t>
-  </si>
-  <si>
-    <t>Education Maintenance Allowance for 2022/23 is displayed as 2023 and for 2024/2025 it is displayed as 2025.</t>
-  </si>
-  <si>
-    <t>Free School Meals: Supplied by West Lothian Council from the SEEMiS database.
-Children in Low Income Families: Accessed from DWP Statxplore.
-Mid Year Population Estimates: National Records of Scotland</t>
-  </si>
-  <si>
-    <t>Free School Meals: Academic years: 2022/23 and 2024/25
-Children in Low Income Families: 2022/23 and 2024/25
-Mid-Year Population Estimates: 2022</t>
-  </si>
-  <si>
-    <t>Clothing Grant: Academic years: 2022/23 and 2024/25
-Children in Low Income Families: 2022/23 and 2024/25
-Mid-Year Population Estimates: 2022</t>
-  </si>
-  <si>
-    <t>Education Maintenance Allowance: Supplied by West Lothian Council from the SEEMiS database.
-Children in Low Income Families: Accessed from DWP Statxplore.
-Mid Year Population Estimates: National Records of Scotland</t>
-  </si>
-  <si>
-    <t>Education Maintenance Allowance: Academic years: 2022/23 and 2024/25
-Children in Low Income Families: 2022/23 and 2024/25
-Mid-Year Population Estimates: 2022</t>
-  </si>
-  <si>
-    <t>Universal Credit: 2025
-Census: 2022</t>
-  </si>
-  <si>
-    <t>The demand measure data does not include in-work households that would be eligible for UC. In the analysis, areas with higher than expected uptake may be influenced by high uptake of UC amongst in-work households.
+    <t>The demand measure data does not include in-work households that would be eligible for UC. In the analysis, areas with higher than estimated uptake may be influenced by high uptake of UC amongst in-work households.
 There is a lag between the data sourced from the census and the UC data, therefore rates are not exact.
 All data is publicly available.</t>
   </si>
-  <si>
-    <t>Universal Credit data is displayed as 2025.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,49 +669,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E1B982-4AAF-471E-AC89-4BA296B3B6F7}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.08203125" customWidth="1"/>
     <col min="2" max="2" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="B1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="126">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="52.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="52" customHeight="1">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="378">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="B5" s="4"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.5">
       <c r="B6" s="5"/>
     </row>
   </sheetData>
@@ -718,16 +725,16 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.77734375" customWidth="1"/>
+    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -743,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -751,7 +758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -759,36 +766,36 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="84">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="70">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="182">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -800,17 +807,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF76746-7DB3-4FD7-9A3F-EF307696AD72}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="29.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -818,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -826,7 +833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -834,7 +841,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -842,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="98">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -850,28 +857,28 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="84">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="42">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="140">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -883,17 +890,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF880852-5D0F-4538-843C-34D9AC4973B7}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.75" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -901,7 +908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -909,7 +916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -917,7 +924,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -925,36 +932,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="140">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="112">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="70">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="168">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -966,17 +973,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D33D3663-F625-404D-9F9A-618D4533EF37}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -984,7 +991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -992,7 +999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1000,7 +1007,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="84">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1016,28 +1023,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="28">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="238">
       <c r="A8" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1049,75 +1056,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3050DF-A96B-49A4-A08C-2F6CF3F579AA}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="273.60000000000002" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="238">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="224">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02355CEA-B782-4497-9D9F-C73FC5FCE064}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="17.9140625" customWidth="1"/>
+    <col min="2" max="2" width="16.9140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1365,6 +1452,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="52e19a84-ae27-4b86-a170-8f47b74f4ad2">
@@ -1373,15 +1469,6 @@
     <TaxCatchAll xmlns="435c4395-9d6a-43e2-b03c-3e7c562397ed" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1404,6 +1491,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477E5E9F-C34A-4BDA-BA59-CD79D5669950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7969E561-3058-4957-B9CB-032DD36D40C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1412,12 +1507,4 @@
     <ds:schemaRef ds:uri="435c4395-9d6a-43e2-b03c-3e7c562397ed"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{477E5E9F-C34A-4BDA-BA59-CD79D5669950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>